<commit_message>
adding recovered files of working prototype to this repo
</commit_message>
<xml_diff>
--- a/Backend/uploads/updated_excel.xlsx
+++ b/Backend/uploads/updated_excel.xlsx
@@ -711,7 +711,7 @@
         <v>DEEP SHARMA</v>
       </c>
       <c r="AX2" t="str">
-        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729624949/legal_documents/iee0pl2ddo2h57766zxm.pdf</v>
+        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729673802/legal_documents/yigucrnc12aszdoju5xl.pdf</v>
       </c>
     </row>
     <row r="3">
@@ -863,7 +863,7 @@
         <v>DEEP SHARMA</v>
       </c>
       <c r="AX3" t="str">
-        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729624949/legal_documents/a7upibdlfifkou5pmno6.pdf</v>
+        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729673803/legal_documents/tqo45nouelxrcupivm3g.pdf</v>
       </c>
     </row>
     <row r="4">
@@ -1015,7 +1015,7 @@
         <v>DEEP SHARMA</v>
       </c>
       <c r="AX4" t="str">
-        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729624948/legal_documents/c5sgwtpancgguhvwrfuj.pdf</v>
+        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729673802/legal_documents/mvtwvae2x63qxi3djhn9.pdf</v>
       </c>
     </row>
     <row r="5">
@@ -1167,7 +1167,7 @@
         <v>DEEP SHARMA</v>
       </c>
       <c r="AX5" t="str">
-        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729624949/legal_documents/n7d8bau6jjn9fcftsjii.pdf</v>
+        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729673802/legal_documents/msordxyihgmk1euwrchd.pdf</v>
       </c>
     </row>
     <row r="6">
@@ -1319,7 +1319,7 @@
         <v>DEEP SHARMA</v>
       </c>
       <c r="AX6" t="str">
-        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729624949/legal_documents/htnuip7bscedrceh7daz.pdf</v>
+        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729673802/legal_documents/vqauzk4fqs9zom7ct5ty.pdf</v>
       </c>
     </row>
     <row r="7">
@@ -1471,7 +1471,7 @@
         <v>DEEP SHARMA</v>
       </c>
       <c r="AX7" t="str">
-        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729624949/legal_documents/ykxhpr8xcnsqemyr0hlz.pdf</v>
+        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729673802/legal_documents/o7cj7ubrarko43r1mykp.pdf</v>
       </c>
     </row>
     <row r="8">
@@ -1623,7 +1623,7 @@
         <v>DEEP SHARMA</v>
       </c>
       <c r="AX8" t="str">
-        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729624949/legal_documents/cfzavringkyhujt7dwfp.pdf</v>
+        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729673803/legal_documents/vbw8dc1ppaf8ume1olbb.pdf</v>
       </c>
     </row>
     <row r="9">
@@ -1775,7 +1775,7 @@
         <v>DEEP SHARMA</v>
       </c>
       <c r="AX9" t="str">
-        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729624948/legal_documents/fmhzudyrqm7pimf5oyna.pdf</v>
+        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729673803/legal_documents/pyppw9rikenx7wonme2k.pdf</v>
       </c>
     </row>
     <row r="10">
@@ -1927,7 +1927,7 @@
         <v>DEEP SHARMA</v>
       </c>
       <c r="AX10" t="str">
-        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729624948/legal_documents/patyxoatvj5ujtyczogy.pdf</v>
+        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729673803/legal_documents/pzk8hkwcveblyiyxxs5g.pdf</v>
       </c>
     </row>
     <row r="11">
@@ -2079,7 +2079,7 @@
         <v>DEEP SHARMA</v>
       </c>
       <c r="AX11" t="str">
-        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729624948/legal_documents/wz7lw1v0k10btefg2f62.pdf</v>
+        <v>https://res.cloudinary.com/dvr6bfzyi/image/upload/v1729673803/legal_documents/oskvugfdx63d1dl6fwdw.pdf</v>
       </c>
     </row>
   </sheetData>

</xml_diff>